<commit_message>
We will have 8 available discounts to set up
Former-commit-id: b6624ba63fd49270c598de28f03d3e5c050eba01
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_DragonDiscounts.xlsx
+++ b/Docs/Content/HungryDragonContent_DragonDiscounts.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ubi\HungryDragon\HD_Client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E076C88-96E1-4EF5-A2FB-D6C5A78752E6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{2D6EDE40-E1AB-43BA-B065-C70EAA8F4172}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="59">
   <si>
     <t>{dragonDiscountsDefinitions}</t>
   </si>
@@ -153,33 +152,18 @@
     <t>&lt;Definition&gt;</t>
   </si>
   <si>
-    <t>dragon_classic</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
     <t>pc</t>
   </si>
   <si>
-    <t>0.25</t>
-  </si>
-  <si>
     <t>2:999</t>
   </si>
   <si>
     <t>dragon_electric</t>
   </si>
   <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>dragon_alien</t>
-  </si>
-  <si>
-    <t>sc</t>
-  </si>
-  <si>
     <t>DragonDiscountOffer1</t>
   </si>
   <si>
@@ -193,15 +177,52 @@
   </si>
   <si>
     <t>2.12</t>
+  </si>
+  <si>
+    <t>dragon_titan</t>
+  </si>
+  <si>
+    <t>nonPayer</t>
+  </si>
+  <si>
+    <t>payer</t>
+  </si>
+  <si>
+    <t>DragonDiscountOffer5</t>
+  </si>
+  <si>
+    <t>DragonDiscountOffer4</t>
+  </si>
+  <si>
+    <t>DragonDiscountOffer6</t>
+  </si>
+  <si>
+    <t>DragonDiscountOffer7</t>
+  </si>
+  <si>
+    <t>DragonDiscountOffer8</t>
+  </si>
+  <si>
+    <t>dragon_dark</t>
+  </si>
+  <si>
+    <t>dragon_skeleton</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="10">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -458,136 +479,305 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="11" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="13" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="11" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="13" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="61">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2222,7 +2412,6 @@
         <sz val="14"/>
         <color auto="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -2257,48 +2446,48 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C8D3503A-B002-4A5D-A196-716575BA2548}" name="Table1" displayName="Table1" ref="B2:AN5" totalsRowShown="0" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43" tableBorderDxfId="41">
-  <autoFilter ref="B2:AN5" xr:uid="{36003FC8-B6FF-4D8D-BEF4-0436769BE4B8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:AN10" totalsRowShown="0" headerRowDxfId="60" dataDxfId="58" headerRowBorderDxfId="59" tableBorderDxfId="57">
+  <autoFilter ref="B2:AN10"/>
   <tableColumns count="39">
-    <tableColumn id="1" xr3:uid="{2637B460-58E7-4993-BFD4-B7EEBCC7E3DC}" name="{dragonDiscountsDefinitions}" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{505B94E9-7AD1-4CA9-914C-F0A7A9A17574}" name="[sku]" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{AC3817CB-518D-4A12-BE24-0A085B55EDE5}" name="[type]" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{99137AD0-D2E1-47EB-B9C6-88A898421314}" name="[enabled]" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{FF9D3CF3-46C9-4680-9B97-47D0F0A695A2}" name="[purchaseLimit]" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{E2FD3F5B-45BF-4403-877E-E367B824834D}" name="[dragonSku]" dataDxfId="35"/>
-    <tableColumn id="7" xr3:uid="{54B962D2-F1FD-4DA2-BD5C-CFF8C89DF5C1}" name="[order]" dataDxfId="34"/>
-    <tableColumn id="8" xr3:uid="{254103B3-5D7D-4E60-8F6C-5EBBF1069620}" name="[refPrice]" dataDxfId="33"/>
-    <tableColumn id="9" xr3:uid="{2A039399-4A8F-4A87-B4B9-5CE9CB10FCAC}" name="[currency]" dataDxfId="32"/>
-    <tableColumn id="10" xr3:uid="{2BF0C061-0CEE-4D6D-89E5-04EC249FDE46}" name="[discount]" dataDxfId="31"/>
-    <tableColumn id="11" xr3:uid="{3D86347F-9B00-4737-8EC4-FE85FFF597BA}" name="[startDate]" dataDxfId="30"/>
-    <tableColumn id="12" xr3:uid="{C54F3F91-C516-41FA-B024-F65CA32957E2}" name="[endDate]" dataDxfId="29"/>
-    <tableColumn id="14" xr3:uid="{A42544A6-784D-4920-B68E-4644885DB1E2}" name="[minAppVersion]" dataDxfId="28"/>
-    <tableColumn id="15" xr3:uid="{1828278D-03FC-4AE8-B4B0-C31E2DF2AD97}" name="[countriesAllowed]" dataDxfId="27"/>
-    <tableColumn id="16" xr3:uid="{36EDDE5A-B518-4A0D-B007-909B0997EB31}" name="[countriesExcluded]" dataDxfId="26"/>
-    <tableColumn id="17" xr3:uid="{4E862B2D-7DE4-40DF-A711-2DC6D9D2AD61}" name="[gamesPlayed]" dataDxfId="25"/>
-    <tableColumn id="18" xr3:uid="{E7BDD77C-BDA3-4ED0-B707-1FDEE768DA12}" name="[payerType]" dataDxfId="24"/>
-    <tableColumn id="19" xr3:uid="{70E3FAEE-B11A-4A60-94DC-B8FC285CB2C0}" name="[minSpent]" dataDxfId="23"/>
-    <tableColumn id="20" xr3:uid="{5D254F4C-3D02-4E76-863C-90FD36462834}" name="[maxSpent]" dataDxfId="22"/>
-    <tableColumn id="21" xr3:uid="{7A66B02B-D1C7-49D9-BF4B-94225C79AA98}" name="[minNumberOfPurchases]" dataDxfId="21"/>
-    <tableColumn id="22" xr3:uid="{CB31DFCE-26A5-465B-B6E2-CEFCCDABF73B}" name="[minutesSinceLastPurchase]" dataDxfId="20"/>
-    <tableColumn id="23" xr3:uid="{65C2E03A-7C84-4F6E-A54E-A03380D54484}" name="[dragonUnlocked]" dataDxfId="19"/>
-    <tableColumn id="24" xr3:uid="{FED265C5-4F6E-4AE9-80B9-80474C6672D4}" name="[dragonOwned]" dataDxfId="18"/>
-    <tableColumn id="25" xr3:uid="{C71F3B1E-094C-4D0B-917F-44A0AB14847A}" name="[dragonNotOwned]" dataDxfId="17"/>
-    <tableColumn id="26" xr3:uid="{C5BD36F7-A637-4203-96B2-ECADE56EFDAF}" name="[scBalanceRange]" dataDxfId="16"/>
-    <tableColumn id="27" xr3:uid="{7C13A7E5-C955-4628-986D-692619A4CBB8}" name="[hcBalanceRange]" dataDxfId="15"/>
-    <tableColumn id="28" xr3:uid="{D47F6EA4-BF51-4E05-BC02-75EFB22159C3}" name="[openedEggs]" dataDxfId="14"/>
-    <tableColumn id="29" xr3:uid="{0B960C2D-7D5C-4418-BABD-F801705DD9EA}" name="[petsOwnedCount]" dataDxfId="13"/>
-    <tableColumn id="30" xr3:uid="{32DC6E8D-E526-473F-97D0-5C953D895C0A}" name="[petsOwned]" dataDxfId="12"/>
-    <tableColumn id="31" xr3:uid="{F37751E1-B9DC-4B80-8516-3A267BEC2267}" name="[petsNotOwned]" dataDxfId="11"/>
-    <tableColumn id="32" xr3:uid="{A64B3654-6562-450E-B58C-013CF498F434}" name="[progressionRange]" dataDxfId="10"/>
-    <tableColumn id="33" xr3:uid="{712008CF-73A3-4398-A850-6598FC7CBA94}" name="[skinsUnlocked]" dataDxfId="9"/>
-    <tableColumn id="34" xr3:uid="{48CC050A-08F1-43FD-A2E5-C54E2124D5DD}" name="[skinsOwned]" dataDxfId="8"/>
-    <tableColumn id="35" xr3:uid="{46AD56A4-635F-41F4-AA41-221221DF204D}" name="[skinsNotOwned]" dataDxfId="7"/>
-    <tableColumn id="36" xr3:uid="{9E24B293-8E9D-4E85-8465-EBE3505AF61F}" name="[maxPurchasePrice]" dataDxfId="6"/>
-    <tableColumn id="37" xr3:uid="{7324EC91-A21E-4735-A7F6-173B38A8D1CE}" name="[lastPurchasePrice]" dataDxfId="5"/>
-    <tableColumn id="38" xr3:uid="{12DD65EA-F111-4B12-956D-D24A4956EE05}" name="[lastPurchaseItemType]" dataDxfId="4"/>
-    <tableColumn id="39" xr3:uid="{DE6F6551-BFB9-4447-AC1B-6FFF1FD5604E}" name="[lastPurchaseItemContent]" dataDxfId="3"/>
-    <tableColumn id="40" xr3:uid="{07C8A679-83DB-4E9E-A79B-235F0E900BDB}" name="[clusterId]" dataDxfId="2"/>
+    <tableColumn id="1" name="{dragonDiscountsDefinitions}" dataDxfId="56"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="55"/>
+    <tableColumn id="3" name="[type]" dataDxfId="54"/>
+    <tableColumn id="4" name="[enabled]" dataDxfId="53"/>
+    <tableColumn id="5" name="[purchaseLimit]" dataDxfId="52"/>
+    <tableColumn id="6" name="[dragonSku]" dataDxfId="51"/>
+    <tableColumn id="7" name="[order]" dataDxfId="50"/>
+    <tableColumn id="8" name="[refPrice]" dataDxfId="49"/>
+    <tableColumn id="9" name="[currency]" dataDxfId="48"/>
+    <tableColumn id="10" name="[discount]" dataDxfId="47"/>
+    <tableColumn id="11" name="[startDate]" dataDxfId="46"/>
+    <tableColumn id="12" name="[endDate]" dataDxfId="45"/>
+    <tableColumn id="14" name="[minAppVersion]" dataDxfId="44"/>
+    <tableColumn id="15" name="[countriesAllowed]" dataDxfId="43"/>
+    <tableColumn id="16" name="[countriesExcluded]" dataDxfId="42"/>
+    <tableColumn id="17" name="[gamesPlayed]" dataDxfId="41"/>
+    <tableColumn id="18" name="[payerType]" dataDxfId="40"/>
+    <tableColumn id="19" name="[minSpent]" dataDxfId="39"/>
+    <tableColumn id="20" name="[maxSpent]" dataDxfId="38"/>
+    <tableColumn id="21" name="[minNumberOfPurchases]" dataDxfId="37"/>
+    <tableColumn id="22" name="[minutesSinceLastPurchase]" dataDxfId="36"/>
+    <tableColumn id="23" name="[dragonUnlocked]" dataDxfId="35"/>
+    <tableColumn id="24" name="[dragonOwned]" dataDxfId="34"/>
+    <tableColumn id="25" name="[dragonNotOwned]" dataDxfId="33"/>
+    <tableColumn id="26" name="[scBalanceRange]" dataDxfId="32"/>
+    <tableColumn id="27" name="[hcBalanceRange]" dataDxfId="31"/>
+    <tableColumn id="28" name="[openedEggs]" dataDxfId="30"/>
+    <tableColumn id="29" name="[petsOwnedCount]" dataDxfId="29"/>
+    <tableColumn id="30" name="[petsOwned]" dataDxfId="28"/>
+    <tableColumn id="31" name="[petsNotOwned]" dataDxfId="27"/>
+    <tableColumn id="32" name="[progressionRange]" dataDxfId="26"/>
+    <tableColumn id="33" name="[skinsUnlocked]" dataDxfId="25"/>
+    <tableColumn id="34" name="[skinsOwned]" dataDxfId="24"/>
+    <tableColumn id="35" name="[skinsNotOwned]" dataDxfId="23"/>
+    <tableColumn id="36" name="[maxPurchasePrice]" dataDxfId="22"/>
+    <tableColumn id="37" name="[lastPurchasePrice]" dataDxfId="21"/>
+    <tableColumn id="38" name="[lastPurchaseItemType]" dataDxfId="20"/>
+    <tableColumn id="39" name="[lastPurchaseItemContent]" dataDxfId="19"/>
+    <tableColumn id="40" name="[clusterId]" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2600,11 +2789,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38B33730-0D3D-423E-8143-EF2D5C7D8530}">
-  <dimension ref="B2:AN5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:AN10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2775,10 +2964,10 @@
         <v>39</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="40" t="s">
-        <v>52</v>
+        <v>44</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>47</v>
       </c>
       <c r="E3" s="12" t="b">
         <v>0</v>
@@ -2787,117 +2976,115 @@
         <v>1</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="H3" s="15">
         <v>1</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="16">
+        <v>99</v>
+      </c>
+      <c r="J3" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="J3" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>43</v>
-      </c>
+      <c r="K3" s="15"/>
       <c r="L3" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="N3" s="38" t="s">
-        <v>53</v>
+        <v>40</v>
+      </c>
+      <c r="N3" s="37" t="s">
+        <v>48</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P3" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q3" s="19">
         <v>2</v>
       </c>
       <c r="R3" s="20" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="S3" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T3" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="U3" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="V3" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W3" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="X3" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y3" s="38" t="s">
-        <v>40</v>
+        <v>40</v>
+      </c>
+      <c r="Y3" s="37" t="s">
+        <v>49</v>
       </c>
       <c r="Z3" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AA3" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AB3" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AC3" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AD3" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AE3" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AF3" s="21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="AG3" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AH3" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AI3" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AJ3" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AK3" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AL3" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AM3" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AN3" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="2:40">
       <c r="B4" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="40" t="s">
-        <v>52</v>
+      <c r="C4" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>47</v>
       </c>
       <c r="E4" s="12" t="b">
         <v>0</v>
@@ -2906,234 +3093,863 @@
         <v>1</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="H4" s="15">
         <v>2</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="16">
+        <v>110</v>
+      </c>
+      <c r="J4" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>46</v>
-      </c>
+      <c r="K4" s="15"/>
       <c r="L4" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M4" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="N4" s="38" t="s">
-        <v>53</v>
+        <v>40</v>
+      </c>
+      <c r="N4" s="37" t="s">
+        <v>48</v>
       </c>
       <c r="O4" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P4" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q4" s="19">
         <v>2</v>
       </c>
       <c r="R4" s="20" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="S4" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T4" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="U4" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="V4" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W4" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="X4" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y4" s="38" t="s">
-        <v>45</v>
+        <v>40</v>
+      </c>
+      <c r="Y4" s="37" t="s">
+        <v>49</v>
       </c>
       <c r="Z4" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AA4" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AB4" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AC4" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AD4" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AE4" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AF4" s="21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="AG4" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AH4" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AI4" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AJ4" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AK4" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AL4" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AM4" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AN4" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="2:40">
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13">
+        <v>1</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="15">
+        <v>3</v>
+      </c>
+      <c r="I5" s="16">
+        <v>60</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="15"/>
+      <c r="L5" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="O5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q5" s="19">
+        <v>2</v>
+      </c>
+      <c r="R5" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="S5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="T5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="U5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="V5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="W5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="X5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y5" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB5" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF5" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN5" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="2:40">
+      <c r="B6" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="13">
+        <v>1</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="15">
+        <v>4</v>
+      </c>
+      <c r="I6" s="16">
+        <v>80</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="15"/>
+      <c r="L6" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="O6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q6" s="19">
+        <v>2</v>
+      </c>
+      <c r="R6" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="S6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="T6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="U6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="V6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="W6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="X6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y6" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB6" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF6" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN6" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="2:40">
+      <c r="B7" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="25" t="b">
+      <c r="D7" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F7" s="26">
         <v>1</v>
       </c>
-      <c r="G5" s="27" t="s">
+      <c r="G7" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" s="28">
+        <v>5</v>
+      </c>
+      <c r="I7" s="29">
+        <v>110</v>
+      </c>
+      <c r="J7" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="28"/>
+      <c r="L7" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="O7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="P7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q7" s="32">
+        <v>2</v>
+      </c>
+      <c r="R7" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="S7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="T7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="U7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="V7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="W7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="X7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y7" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB7" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF7" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN7" s="35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:40">
+      <c r="B8" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="28">
-        <v>3</v>
-      </c>
-      <c r="I5" s="29" t="s">
+      <c r="E8" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="26">
+        <v>1</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="28">
+        <v>6</v>
+      </c>
+      <c r="I8" s="29">
+        <v>250</v>
+      </c>
+      <c r="J8" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="29" t="s">
+      <c r="K8" s="28"/>
+      <c r="L8" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="M8" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="K5" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="L5" s="30" t="s">
+      <c r="O8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="P8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q8" s="32">
+        <v>2</v>
+      </c>
+      <c r="R8" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="S8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="T8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="U8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="V8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="W8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="X8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y8" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB8" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF8" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN8" s="35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="2:40">
+      <c r="B9" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="13">
+        <v>1</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="15">
+        <v>7</v>
+      </c>
+      <c r="I9" s="16">
+        <v>110</v>
+      </c>
+      <c r="J9" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="31" t="s">
+      <c r="K9" s="15"/>
+      <c r="L9" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="M9" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="N9" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="O9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="P9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q9" s="19">
+        <v>2</v>
+      </c>
+      <c r="R9" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="S9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="T9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="U9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="V9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="W9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="X9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y9" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB9" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF9" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN9" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="2:40">
+      <c r="B10" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="26">
+        <v>1</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="28">
+        <v>8</v>
+      </c>
+      <c r="I10" s="29">
+        <v>250</v>
+      </c>
+      <c r="J10" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="N5" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="O5" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="P5" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q5" s="32">
+      <c r="K10" s="28"/>
+      <c r="L10" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="M10" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="O10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="P10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q10" s="32">
         <v>2</v>
       </c>
-      <c r="R5" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="S5" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="T5" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="U5" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="V5" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="W5" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="X5" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y5" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z5" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA5" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB5" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC5" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD5" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="AE5" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="AF5" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="AG5" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH5" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI5" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ5" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="AK5" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="AL5" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM5" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="AN5" s="35" t="s">
-        <v>41</v>
+      <c r="R10" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="S10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="T10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="U10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="V10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="W10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="X10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y10" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB10" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF10" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN10" s="35" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E3:E5">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="E3 E5">
+    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",E3)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",E3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",E4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",E4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",E6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",E6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",E7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",E7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",E8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",E8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",E9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",E9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",E10)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",E3)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",E10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Dragon Discounts: Content - Added segmentation by player source.
Former-commit-id: f2688126cb7c231d8492456799207634980dded2
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_DragonDiscounts.xlsx
+++ b/Docs/Content/HungryDragonContent_DragonDiscounts.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ubi\HungryDragon\HD_Client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBF5969-447A-45A9-BBDC-3792DD504271}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21840"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="60">
   <si>
     <t>{dragonDiscountsDefinitions}</t>
   </si>
@@ -207,12 +202,15 @@
   </si>
   <si>
     <t>dragon_skeleton</t>
+  </si>
+  <si>
+    <t>[playerSources]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10">
     <font>
       <sz val="12"/>
@@ -617,46 +615,44 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="61">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+  <dxfs count="58">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2446,48 +2442,49 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:AN10" totalsRowShown="0" headerRowDxfId="60" dataDxfId="58" headerRowBorderDxfId="59" tableBorderDxfId="57">
-  <autoFilter ref="B2:AN10"/>
-  <tableColumns count="39">
-    <tableColumn id="1" name="{dragonDiscountsDefinitions}" dataDxfId="56"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="55"/>
-    <tableColumn id="3" name="[type]" dataDxfId="54"/>
-    <tableColumn id="4" name="[enabled]" dataDxfId="53"/>
-    <tableColumn id="5" name="[purchaseLimit]" dataDxfId="52"/>
-    <tableColumn id="6" name="[dragonSku]" dataDxfId="51"/>
-    <tableColumn id="7" name="[order]" dataDxfId="50"/>
-    <tableColumn id="8" name="[refPrice]" dataDxfId="49"/>
-    <tableColumn id="9" name="[currency]" dataDxfId="48"/>
-    <tableColumn id="10" name="[discount]" dataDxfId="47"/>
-    <tableColumn id="11" name="[startDate]" dataDxfId="46"/>
-    <tableColumn id="12" name="[endDate]" dataDxfId="45"/>
-    <tableColumn id="14" name="[minAppVersion]" dataDxfId="44"/>
-    <tableColumn id="15" name="[countriesAllowed]" dataDxfId="43"/>
-    <tableColumn id="16" name="[countriesExcluded]" dataDxfId="42"/>
-    <tableColumn id="17" name="[gamesPlayed]" dataDxfId="41"/>
-    <tableColumn id="18" name="[payerType]" dataDxfId="40"/>
-    <tableColumn id="19" name="[minSpent]" dataDxfId="39"/>
-    <tableColumn id="20" name="[maxSpent]" dataDxfId="38"/>
-    <tableColumn id="21" name="[minNumberOfPurchases]" dataDxfId="37"/>
-    <tableColumn id="22" name="[minutesSinceLastPurchase]" dataDxfId="36"/>
-    <tableColumn id="23" name="[dragonUnlocked]" dataDxfId="35"/>
-    <tableColumn id="24" name="[dragonOwned]" dataDxfId="34"/>
-    <tableColumn id="25" name="[dragonNotOwned]" dataDxfId="33"/>
-    <tableColumn id="26" name="[scBalanceRange]" dataDxfId="32"/>
-    <tableColumn id="27" name="[hcBalanceRange]" dataDxfId="31"/>
-    <tableColumn id="28" name="[openedEggs]" dataDxfId="30"/>
-    <tableColumn id="29" name="[petsOwnedCount]" dataDxfId="29"/>
-    <tableColumn id="30" name="[petsOwned]" dataDxfId="28"/>
-    <tableColumn id="31" name="[petsNotOwned]" dataDxfId="27"/>
-    <tableColumn id="32" name="[progressionRange]" dataDxfId="26"/>
-    <tableColumn id="33" name="[skinsUnlocked]" dataDxfId="25"/>
-    <tableColumn id="34" name="[skinsOwned]" dataDxfId="24"/>
-    <tableColumn id="35" name="[skinsNotOwned]" dataDxfId="23"/>
-    <tableColumn id="36" name="[maxPurchasePrice]" dataDxfId="22"/>
-    <tableColumn id="37" name="[lastPurchasePrice]" dataDxfId="21"/>
-    <tableColumn id="38" name="[lastPurchaseItemType]" dataDxfId="20"/>
-    <tableColumn id="39" name="[lastPurchaseItemContent]" dataDxfId="19"/>
-    <tableColumn id="40" name="[clusterId]" dataDxfId="18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B2:AO10" totalsRowShown="0" headerRowDxfId="57" dataDxfId="55" headerRowBorderDxfId="56" tableBorderDxfId="54">
+  <autoFilter ref="B2:AO10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="40">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{dragonDiscountsDefinitions}" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[type]" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[enabled]" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[purchaseLimit]" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[dragonSku]" dataDxfId="48"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[order]" dataDxfId="47"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[refPrice]" dataDxfId="46"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[currency]" dataDxfId="45"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[discount]" dataDxfId="44"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[startDate]" dataDxfId="43"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="[endDate]" dataDxfId="42"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="[minAppVersion]" dataDxfId="41"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[countriesAllowed]" dataDxfId="40"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[countriesExcluded]" dataDxfId="39"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="[gamesPlayed]" dataDxfId="38"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="[payerType]" dataDxfId="37"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="[minSpent]" dataDxfId="36"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="[maxSpent]" dataDxfId="35"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="[minNumberOfPurchases]" dataDxfId="34"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="[minutesSinceLastPurchase]" dataDxfId="33"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="[dragonUnlocked]" dataDxfId="32"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="[dragonOwned]" dataDxfId="31"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="[dragonNotOwned]" dataDxfId="30"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="[scBalanceRange]" dataDxfId="29"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="[hcBalanceRange]" dataDxfId="28"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="[openedEggs]" dataDxfId="27"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="[petsOwnedCount]" dataDxfId="26"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="[petsOwned]" dataDxfId="25"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="[petsNotOwned]" dataDxfId="24"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="[progressionRange]" dataDxfId="23"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="[skinsUnlocked]" dataDxfId="22"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="[skinsOwned]" dataDxfId="21"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="[skinsNotOwned]" dataDxfId="20"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="[maxPurchasePrice]" dataDxfId="19"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="[lastPurchasePrice]" dataDxfId="18"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="[lastPurchaseItemType]" dataDxfId="17"/>
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="[lastPurchaseItemContent]" dataDxfId="16"/>
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="[clusterId]" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{C3357C0B-3974-426A-9EA4-744A32EAC7BE}" name="[playerSources]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2789,11 +2786,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AN10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:AO10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AO22" sqref="AO22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2837,10 +2834,10 @@
     <col min="38" max="38" width="21.875" customWidth="1"/>
     <col min="39" max="39" width="26.25" customWidth="1"/>
     <col min="40" max="40" width="29.5" customWidth="1"/>
-    <col min="41" max="41" width="13" customWidth="1"/>
+    <col min="41" max="41" width="28.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:40" ht="149.1" customHeight="1">
+    <row r="2" spans="2:41" ht="149.1" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2958,8 +2955,11 @@
       <c r="AN2" s="22" t="s">
         <v>38</v>
       </c>
+      <c r="AO2" s="9" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="3" spans="2:40">
+    <row r="3" spans="2:41">
       <c r="B3" s="11" t="s">
         <v>39</v>
       </c>
@@ -3075,8 +3075,11 @@
       <c r="AN3" s="23" t="s">
         <v>40</v>
       </c>
+      <c r="AO3" s="23" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="4" spans="2:40">
+    <row r="4" spans="2:41">
       <c r="B4" s="11" t="s">
         <v>39</v>
       </c>
@@ -3192,8 +3195,11 @@
       <c r="AN4" s="23" t="s">
         <v>40</v>
       </c>
+      <c r="AO4" s="23" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="5" spans="2:40">
+    <row r="5" spans="2:41">
       <c r="B5" s="11" t="s">
         <v>39</v>
       </c>
@@ -3309,8 +3315,11 @@
       <c r="AN5" s="23" t="s">
         <v>40</v>
       </c>
+      <c r="AO5" s="23" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="6" spans="2:40">
+    <row r="6" spans="2:41">
       <c r="B6" s="11" t="s">
         <v>39</v>
       </c>
@@ -3426,8 +3435,11 @@
       <c r="AN6" s="23" t="s">
         <v>40</v>
       </c>
+      <c r="AO6" s="23" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="7" spans="2:40">
+    <row r="7" spans="2:41">
       <c r="B7" s="24" t="s">
         <v>39</v>
       </c>
@@ -3543,8 +3555,11 @@
       <c r="AN7" s="35" t="s">
         <v>40</v>
       </c>
+      <c r="AO7" s="35" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="8" spans="2:40">
+    <row r="8" spans="2:41">
       <c r="B8" s="24" t="s">
         <v>39</v>
       </c>
@@ -3660,8 +3675,11 @@
       <c r="AN8" s="35" t="s">
         <v>40</v>
       </c>
+      <c r="AO8" s="35" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="9" spans="2:40">
+    <row r="9" spans="2:41">
       <c r="B9" s="11" t="s">
         <v>39</v>
       </c>
@@ -3777,8 +3795,11 @@
       <c r="AN9" s="23" t="s">
         <v>40</v>
       </c>
+      <c r="AO9" s="23" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="10" spans="2:40">
+    <row r="10" spans="2:41">
       <c r="B10" s="24" t="s">
         <v>39</v>
       </c>
@@ -3892,63 +3913,66 @@
         <v>40</v>
       </c>
       <c r="AN10" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="AO10" s="35" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E3 E5">
-    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="14" priority="17" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="13" priority="18" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",E4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",E4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="10" priority="13" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="9" priority="14" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",E6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",E7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",E8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",E10)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added uniqueId column ( https://confluence.ubisoft.com/pages/viewpage.action?pageId=872683518 )
Former-commit-id: 066004e3574c1a189a475b61778e1a048cdcd9ae
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_DragonDiscounts.xlsx
+++ b/Docs/Content/HungryDragonContent_DragonDiscounts.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ubi\HungryDragon\HD_Client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBF5969-447A-45A9-BBDC-3792DD504271}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="61">
   <si>
     <t>{dragonDiscountsDefinitions}</t>
   </si>
@@ -205,12 +204,15 @@
   </si>
   <si>
     <t>[playerSources]</t>
+  </si>
+  <si>
+    <t>[uniqueId]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10">
     <font>
       <sz val="12"/>
@@ -477,7 +479,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
@@ -610,12 +612,198 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="58">
+  <dxfs count="59">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -653,146 +841,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2442,49 +2490,50 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B2:AO10" totalsRowShown="0" headerRowDxfId="57" dataDxfId="55" headerRowBorderDxfId="56" tableBorderDxfId="54">
-  <autoFilter ref="B2:AO10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="40">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{dragonDiscountsDefinitions}" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[type]" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[enabled]" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[purchaseLimit]" dataDxfId="49"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[dragonSku]" dataDxfId="48"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[order]" dataDxfId="47"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[refPrice]" dataDxfId="46"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[currency]" dataDxfId="45"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[discount]" dataDxfId="44"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[startDate]" dataDxfId="43"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="[endDate]" dataDxfId="42"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="[minAppVersion]" dataDxfId="41"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[countriesAllowed]" dataDxfId="40"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[countriesExcluded]" dataDxfId="39"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="[gamesPlayed]" dataDxfId="38"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="[payerType]" dataDxfId="37"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="[minSpent]" dataDxfId="36"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="[maxSpent]" dataDxfId="35"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="[minNumberOfPurchases]" dataDxfId="34"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="[minutesSinceLastPurchase]" dataDxfId="33"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="[dragonUnlocked]" dataDxfId="32"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="[dragonOwned]" dataDxfId="31"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="[dragonNotOwned]" dataDxfId="30"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="[scBalanceRange]" dataDxfId="29"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="[hcBalanceRange]" dataDxfId="28"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="[openedEggs]" dataDxfId="27"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="[petsOwnedCount]" dataDxfId="26"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="[petsOwned]" dataDxfId="25"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="[petsNotOwned]" dataDxfId="24"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="[progressionRange]" dataDxfId="23"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="[skinsUnlocked]" dataDxfId="22"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="[skinsOwned]" dataDxfId="21"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="[skinsNotOwned]" dataDxfId="20"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="[maxPurchasePrice]" dataDxfId="19"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="[lastPurchasePrice]" dataDxfId="18"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="[lastPurchaseItemType]" dataDxfId="17"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="[lastPurchaseItemContent]" dataDxfId="16"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="[clusterId]" dataDxfId="15"/>
-    <tableColumn id="13" xr3:uid="{C3357C0B-3974-426A-9EA4-744A32EAC7BE}" name="[playerSources]" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:AP10" totalsRowShown="0" headerRowDxfId="58" dataDxfId="56" headerRowBorderDxfId="57" tableBorderDxfId="55">
+  <autoFilter ref="B2:AP10"/>
+  <tableColumns count="41">
+    <tableColumn id="1" name="{dragonDiscountsDefinitions}" dataDxfId="54"/>
+    <tableColumn id="41" name="[uniqueId]" dataDxfId="0"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="53"/>
+    <tableColumn id="3" name="[type]" dataDxfId="52"/>
+    <tableColumn id="4" name="[enabled]" dataDxfId="51"/>
+    <tableColumn id="5" name="[purchaseLimit]" dataDxfId="50"/>
+    <tableColumn id="6" name="[dragonSku]" dataDxfId="49"/>
+    <tableColumn id="7" name="[order]" dataDxfId="48"/>
+    <tableColumn id="8" name="[refPrice]" dataDxfId="47"/>
+    <tableColumn id="9" name="[currency]" dataDxfId="46"/>
+    <tableColumn id="10" name="[discount]" dataDxfId="45"/>
+    <tableColumn id="11" name="[startDate]" dataDxfId="44"/>
+    <tableColumn id="12" name="[endDate]" dataDxfId="43"/>
+    <tableColumn id="14" name="[minAppVersion]" dataDxfId="42"/>
+    <tableColumn id="15" name="[countriesAllowed]" dataDxfId="41"/>
+    <tableColumn id="16" name="[countriesExcluded]" dataDxfId="40"/>
+    <tableColumn id="17" name="[gamesPlayed]" dataDxfId="39"/>
+    <tableColumn id="18" name="[payerType]" dataDxfId="38"/>
+    <tableColumn id="19" name="[minSpent]" dataDxfId="37"/>
+    <tableColumn id="20" name="[maxSpent]" dataDxfId="36"/>
+    <tableColumn id="21" name="[minNumberOfPurchases]" dataDxfId="35"/>
+    <tableColumn id="22" name="[minutesSinceLastPurchase]" dataDxfId="34"/>
+    <tableColumn id="23" name="[dragonUnlocked]" dataDxfId="33"/>
+    <tableColumn id="24" name="[dragonOwned]" dataDxfId="32"/>
+    <tableColumn id="25" name="[dragonNotOwned]" dataDxfId="31"/>
+    <tableColumn id="26" name="[scBalanceRange]" dataDxfId="30"/>
+    <tableColumn id="27" name="[hcBalanceRange]" dataDxfId="29"/>
+    <tableColumn id="28" name="[openedEggs]" dataDxfId="28"/>
+    <tableColumn id="29" name="[petsOwnedCount]" dataDxfId="27"/>
+    <tableColumn id="30" name="[petsOwned]" dataDxfId="26"/>
+    <tableColumn id="31" name="[petsNotOwned]" dataDxfId="25"/>
+    <tableColumn id="32" name="[progressionRange]" dataDxfId="24"/>
+    <tableColumn id="33" name="[skinsUnlocked]" dataDxfId="23"/>
+    <tableColumn id="34" name="[skinsOwned]" dataDxfId="22"/>
+    <tableColumn id="35" name="[skinsNotOwned]" dataDxfId="21"/>
+    <tableColumn id="36" name="[maxPurchasePrice]" dataDxfId="20"/>
+    <tableColumn id="37" name="[lastPurchasePrice]" dataDxfId="19"/>
+    <tableColumn id="38" name="[lastPurchaseItemType]" dataDxfId="18"/>
+    <tableColumn id="39" name="[lastPurchaseItemContent]" dataDxfId="17"/>
+    <tableColumn id="40" name="[clusterId]" dataDxfId="16"/>
+    <tableColumn id="13" name="[playerSources]" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2786,232 +2835,235 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:AO10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:AP10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AO22" sqref="AO22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="31.125" customWidth="1"/>
-    <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="4" width="20.375" customWidth="1"/>
-    <col min="5" max="5" width="12.25" customWidth="1"/>
-    <col min="6" max="6" width="18.25" customWidth="1"/>
-    <col min="7" max="7" width="28.375" customWidth="1"/>
-    <col min="8" max="8" width="9.75" customWidth="1"/>
-    <col min="9" max="9" width="12.125" customWidth="1"/>
-    <col min="10" max="10" width="12.875" customWidth="1"/>
-    <col min="11" max="11" width="12.75" customWidth="1"/>
-    <col min="12" max="12" width="13.75" customWidth="1"/>
-    <col min="13" max="13" width="12.75" customWidth="1"/>
-    <col min="14" max="14" width="21.125" customWidth="1"/>
-    <col min="15" max="15" width="19.625" customWidth="1"/>
-    <col min="16" max="16" width="21.875" customWidth="1"/>
-    <col min="17" max="17" width="22.5" customWidth="1"/>
-    <col min="18" max="18" width="17.25" customWidth="1"/>
-    <col min="19" max="19" width="14.625" customWidth="1"/>
-    <col min="20" max="20" width="13.75" customWidth="1"/>
-    <col min="21" max="21" width="14.125" customWidth="1"/>
-    <col min="22" max="22" width="28.5" customWidth="1"/>
-    <col min="23" max="23" width="30.625" customWidth="1"/>
-    <col min="24" max="24" width="20.375" customWidth="1"/>
-    <col min="25" max="25" width="18.25" customWidth="1"/>
-    <col min="26" max="26" width="22" customWidth="1"/>
-    <col min="27" max="27" width="20.125" customWidth="1"/>
-    <col min="28" max="28" width="20.375" customWidth="1"/>
-    <col min="29" max="29" width="16.125" customWidth="1"/>
-    <col min="30" max="30" width="21.625" customWidth="1"/>
-    <col min="31" max="31" width="15.75" customWidth="1"/>
-    <col min="32" max="32" width="19.5" customWidth="1"/>
-    <col min="33" max="33" width="22.125" customWidth="1"/>
-    <col min="34" max="34" width="18.5" customWidth="1"/>
-    <col min="35" max="35" width="16.375" customWidth="1"/>
-    <col min="36" max="36" width="20.125" customWidth="1"/>
-    <col min="37" max="37" width="22.375" customWidth="1"/>
-    <col min="38" max="38" width="21.875" customWidth="1"/>
-    <col min="39" max="39" width="26.25" customWidth="1"/>
-    <col min="40" max="40" width="29.5" customWidth="1"/>
-    <col min="41" max="41" width="28.625" customWidth="1"/>
+    <col min="2" max="3" width="31.125" customWidth="1"/>
+    <col min="4" max="4" width="19.5" customWidth="1"/>
+    <col min="5" max="5" width="20.375" customWidth="1"/>
+    <col min="6" max="6" width="12.25" customWidth="1"/>
+    <col min="7" max="7" width="18.25" customWidth="1"/>
+    <col min="8" max="8" width="28.375" customWidth="1"/>
+    <col min="9" max="9" width="9.75" customWidth="1"/>
+    <col min="10" max="10" width="12.125" customWidth="1"/>
+    <col min="11" max="11" width="12.875" customWidth="1"/>
+    <col min="12" max="12" width="12.75" customWidth="1"/>
+    <col min="13" max="13" width="13.75" customWidth="1"/>
+    <col min="14" max="14" width="12.75" customWidth="1"/>
+    <col min="15" max="15" width="21.125" customWidth="1"/>
+    <col min="16" max="16" width="19.625" customWidth="1"/>
+    <col min="17" max="17" width="21.875" customWidth="1"/>
+    <col min="18" max="18" width="22.5" customWidth="1"/>
+    <col min="19" max="19" width="17.25" customWidth="1"/>
+    <col min="20" max="20" width="14.625" customWidth="1"/>
+    <col min="21" max="21" width="13.75" customWidth="1"/>
+    <col min="22" max="22" width="14.125" customWidth="1"/>
+    <col min="23" max="23" width="28.5" customWidth="1"/>
+    <col min="24" max="24" width="30.625" customWidth="1"/>
+    <col min="25" max="25" width="20.375" customWidth="1"/>
+    <col min="26" max="26" width="18.25" customWidth="1"/>
+    <col min="27" max="27" width="22" customWidth="1"/>
+    <col min="28" max="28" width="20.125" customWidth="1"/>
+    <col min="29" max="29" width="20.375" customWidth="1"/>
+    <col min="30" max="30" width="16.125" customWidth="1"/>
+    <col min="31" max="31" width="21.625" customWidth="1"/>
+    <col min="32" max="32" width="15.75" customWidth="1"/>
+    <col min="33" max="33" width="19.5" customWidth="1"/>
+    <col min="34" max="34" width="22.125" customWidth="1"/>
+    <col min="35" max="35" width="18.5" customWidth="1"/>
+    <col min="36" max="36" width="16.375" customWidth="1"/>
+    <col min="37" max="37" width="20.125" customWidth="1"/>
+    <col min="38" max="38" width="22.375" customWidth="1"/>
+    <col min="39" max="39" width="21.875" customWidth="1"/>
+    <col min="40" max="40" width="26.25" customWidth="1"/>
+    <col min="41" max="41" width="29.5" customWidth="1"/>
+    <col min="42" max="42" width="28.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:41" ht="149.1" customHeight="1">
+    <row r="2" spans="2:42" ht="149.1" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="M2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="N2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="T2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="U2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="V2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="W2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="W2" s="9" t="s">
+      <c r="X2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="X2" s="9" t="s">
+      <c r="Y2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="Y2" s="9" t="s">
+      <c r="Z2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="Z2" s="9" t="s">
+      <c r="AA2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="AA2" s="9" t="s">
+      <c r="AB2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="AB2" s="9" t="s">
+      <c r="AC2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" s="9" t="s">
+      <c r="AD2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="AD2" s="9" t="s">
+      <c r="AE2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AE2" s="9" t="s">
+      <c r="AF2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="AF2" s="9" t="s">
+      <c r="AG2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="9" t="s">
+      <c r="AH2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="9" t="s">
+      <c r="AI2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="AI2" s="10" t="s">
+      <c r="AJ2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="AJ2" s="9" t="s">
+      <c r="AK2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AK2" s="9" t="s">
+      <c r="AL2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="AL2" s="9" t="s">
+      <c r="AM2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="AM2" s="9" t="s">
+      <c r="AN2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AN2" s="22" t="s">
+      <c r="AO2" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="AO2" s="9" t="s">
+      <c r="AP2" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="2:41">
+    <row r="3" spans="2:42">
       <c r="B3" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="E3" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="12" t="b">
+      <c r="F3" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="F3" s="13">
+      <c r="G3" s="13">
         <v>1</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="H3" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H3" s="15">
+      <c r="I3" s="15">
         <v>1</v>
       </c>
-      <c r="I3" s="16">
+      <c r="J3" s="16">
         <v>99</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="K3" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="15"/>
-      <c r="L3" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="M3" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="N3" s="37" t="s">
+      <c r="L3" s="15"/>
+      <c r="M3" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="O3" s="19" t="s">
-        <v>40</v>
-      </c>
       <c r="P3" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="Q3" s="19">
+      <c r="Q3" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="19">
         <v>2</v>
       </c>
-      <c r="R3" s="20" t="s">
+      <c r="S3" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="S3" s="19" t="s">
-        <v>40</v>
-      </c>
       <c r="T3" s="19" t="s">
         <v>40</v>
       </c>
@@ -3027,19 +3079,19 @@
       <c r="X3" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="Y3" s="37" t="s">
+      <c r="Y3" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z3" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="Z3" s="19" t="s">
-        <v>40</v>
-      </c>
       <c r="AA3" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="AB3" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC3" s="19" t="s">
+      <c r="AB3" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC3" s="20" t="s">
         <v>40</v>
       </c>
       <c r="AD3" s="19" t="s">
@@ -3048,12 +3100,12 @@
       <c r="AE3" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="AF3" s="21" t="s">
+      <c r="AF3" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG3" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="AG3" s="19" t="s">
-        <v>40</v>
-      </c>
       <c r="AH3" s="19" t="s">
         <v>40</v>
       </c>
@@ -3072,66 +3124,69 @@
       <c r="AM3" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="AN3" s="23" t="s">
+      <c r="AN3" s="19" t="s">
         <v>40</v>
       </c>
       <c r="AO3" s="23" t="s">
         <v>40</v>
       </c>
+      <c r="AP3" s="23" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="4" spans="2:41">
+    <row r="4" spans="2:42">
       <c r="B4" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="E4" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="12" t="b">
+      <c r="F4" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="F4" s="13">
+      <c r="G4" s="13">
         <v>1</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="H4" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="15">
+      <c r="I4" s="15">
         <v>2</v>
       </c>
-      <c r="I4" s="16">
+      <c r="J4" s="16">
         <v>110</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="K4" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="K4" s="15"/>
-      <c r="L4" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="M4" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" s="37" t="s">
+      <c r="L4" s="15"/>
+      <c r="M4" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="O4" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="O4" s="19" t="s">
-        <v>40</v>
-      </c>
       <c r="P4" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="Q4" s="19">
+      <c r="Q4" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="R4" s="19">
         <v>2</v>
       </c>
-      <c r="R4" s="20" t="s">
+      <c r="S4" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="S4" s="19" t="s">
-        <v>40</v>
-      </c>
       <c r="T4" s="19" t="s">
         <v>40</v>
       </c>
@@ -3147,19 +3202,19 @@
       <c r="X4" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="Y4" s="37" t="s">
+      <c r="Y4" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z4" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="Z4" s="19" t="s">
-        <v>40</v>
-      </c>
       <c r="AA4" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="AB4" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC4" s="19" t="s">
+      <c r="AB4" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC4" s="20" t="s">
         <v>40</v>
       </c>
       <c r="AD4" s="19" t="s">
@@ -3168,12 +3223,12 @@
       <c r="AE4" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="AF4" s="21" t="s">
+      <c r="AF4" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG4" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="AG4" s="19" t="s">
-        <v>40</v>
-      </c>
       <c r="AH4" s="19" t="s">
         <v>40</v>
       </c>
@@ -3192,66 +3247,69 @@
       <c r="AM4" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="AN4" s="23" t="s">
+      <c r="AN4" s="19" t="s">
         <v>40</v>
       </c>
       <c r="AO4" s="23" t="s">
         <v>40</v>
       </c>
+      <c r="AP4" s="23" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="5" spans="2:41">
+    <row r="5" spans="2:42">
       <c r="B5" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="E5" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="12" t="b">
+      <c r="F5" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="F5" s="13">
+      <c r="G5" s="13">
         <v>1</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="H5" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="15">
+      <c r="I5" s="15">
         <v>3</v>
       </c>
-      <c r="I5" s="16">
+      <c r="J5" s="16">
         <v>60</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="K5" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="K5" s="15"/>
-      <c r="L5" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="M5" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="N5" s="37" t="s">
+      <c r="L5" s="15"/>
+      <c r="M5" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="O5" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="O5" s="19" t="s">
-        <v>40</v>
-      </c>
       <c r="P5" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="Q5" s="19">
+      <c r="Q5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="R5" s="19">
         <v>2</v>
       </c>
-      <c r="R5" s="20" t="s">
+      <c r="S5" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="S5" s="19" t="s">
-        <v>40</v>
-      </c>
       <c r="T5" s="19" t="s">
         <v>40</v>
       </c>
@@ -3267,19 +3325,19 @@
       <c r="X5" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="Y5" s="37" t="s">
+      <c r="Y5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z5" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="Z5" s="19" t="s">
-        <v>40</v>
-      </c>
       <c r="AA5" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="AB5" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC5" s="19" t="s">
+      <c r="AB5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC5" s="20" t="s">
         <v>40</v>
       </c>
       <c r="AD5" s="19" t="s">
@@ -3288,12 +3346,12 @@
       <c r="AE5" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="AF5" s="21" t="s">
+      <c r="AF5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG5" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="AG5" s="19" t="s">
-        <v>40</v>
-      </c>
       <c r="AH5" s="19" t="s">
         <v>40</v>
       </c>
@@ -3312,66 +3370,69 @@
       <c r="AM5" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="AN5" s="23" t="s">
+      <c r="AN5" s="19" t="s">
         <v>40</v>
       </c>
       <c r="AO5" s="23" t="s">
         <v>40</v>
       </c>
+      <c r="AP5" s="23" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="6" spans="2:41">
+    <row r="6" spans="2:42">
       <c r="B6" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="E6" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="12" t="b">
+      <c r="F6" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="F6" s="13">
+      <c r="G6" s="13">
         <v>1</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="H6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="15">
+      <c r="I6" s="15">
         <v>4</v>
       </c>
-      <c r="I6" s="16">
+      <c r="J6" s="16">
         <v>80</v>
       </c>
-      <c r="J6" s="16" t="s">
+      <c r="K6" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="15"/>
-      <c r="L6" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="M6" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="N6" s="37" t="s">
+      <c r="L6" s="15"/>
+      <c r="M6" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="O6" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="O6" s="19" t="s">
-        <v>40</v>
-      </c>
       <c r="P6" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="Q6" s="19">
+      <c r="Q6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="R6" s="19">
         <v>2</v>
       </c>
-      <c r="R6" s="20" t="s">
+      <c r="S6" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="S6" s="19" t="s">
-        <v>40</v>
-      </c>
       <c r="T6" s="19" t="s">
         <v>40</v>
       </c>
@@ -3387,19 +3448,19 @@
       <c r="X6" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="Y6" s="37" t="s">
+      <c r="Y6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z6" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="Z6" s="19" t="s">
-        <v>40</v>
-      </c>
       <c r="AA6" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="AB6" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC6" s="19" t="s">
+      <c r="AB6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC6" s="20" t="s">
         <v>40</v>
       </c>
       <c r="AD6" s="19" t="s">
@@ -3408,12 +3469,12 @@
       <c r="AE6" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="AF6" s="21" t="s">
+      <c r="AF6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG6" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="AG6" s="19" t="s">
-        <v>40</v>
-      </c>
       <c r="AH6" s="19" t="s">
         <v>40</v>
       </c>
@@ -3432,66 +3493,69 @@
       <c r="AM6" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="AN6" s="23" t="s">
+      <c r="AN6" s="19" t="s">
         <v>40</v>
       </c>
       <c r="AO6" s="23" t="s">
         <v>40</v>
       </c>
+      <c r="AP6" s="23" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="7" spans="2:41">
+    <row r="7" spans="2:42">
       <c r="B7" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="E7" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="12" t="b">
+      <c r="F7" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="F7" s="26">
+      <c r="G7" s="26">
         <v>1</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="H7" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="H7" s="28">
+      <c r="I7" s="28">
         <v>5</v>
       </c>
-      <c r="I7" s="29">
+      <c r="J7" s="29">
         <v>110</v>
       </c>
-      <c r="J7" s="29" t="s">
+      <c r="K7" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="28"/>
-      <c r="L7" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="M7" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="N7" s="38" t="s">
+      <c r="L7" s="28"/>
+      <c r="M7" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="O7" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="O7" s="32" t="s">
-        <v>40</v>
-      </c>
       <c r="P7" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="Q7" s="32">
+      <c r="Q7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="R7" s="32">
         <v>2</v>
       </c>
-      <c r="R7" s="33" t="s">
+      <c r="S7" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="S7" s="32" t="s">
-        <v>40</v>
-      </c>
       <c r="T7" s="32" t="s">
         <v>40</v>
       </c>
@@ -3507,19 +3571,19 @@
       <c r="X7" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="Y7" s="38" t="s">
+      <c r="Y7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z7" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="Z7" s="32" t="s">
-        <v>40</v>
-      </c>
       <c r="AA7" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="AB7" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC7" s="32" t="s">
+      <c r="AB7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC7" s="33" t="s">
         <v>40</v>
       </c>
       <c r="AD7" s="32" t="s">
@@ -3528,12 +3592,12 @@
       <c r="AE7" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="AF7" s="34" t="s">
+      <c r="AF7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG7" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="AG7" s="32" t="s">
-        <v>40</v>
-      </c>
       <c r="AH7" s="32" t="s">
         <v>40</v>
       </c>
@@ -3552,66 +3616,69 @@
       <c r="AM7" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="AN7" s="35" t="s">
+      <c r="AN7" s="32" t="s">
         <v>40</v>
       </c>
       <c r="AO7" s="35" t="s">
         <v>40</v>
       </c>
+      <c r="AP7" s="35" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="8" spans="2:41">
+    <row r="8" spans="2:42">
       <c r="B8" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="E8" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="12" t="b">
+      <c r="F8" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="F8" s="26">
+      <c r="G8" s="26">
         <v>1</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="H8" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="H8" s="28">
+      <c r="I8" s="28">
         <v>6</v>
       </c>
-      <c r="I8" s="29">
+      <c r="J8" s="29">
         <v>250</v>
       </c>
-      <c r="J8" s="29" t="s">
+      <c r="K8" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="K8" s="28"/>
-      <c r="L8" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="M8" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="N8" s="32" t="s">
+      <c r="L8" s="28"/>
+      <c r="M8" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="O8" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="O8" s="32" t="s">
-        <v>40</v>
-      </c>
       <c r="P8" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="Q8" s="32">
+      <c r="Q8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="R8" s="32">
         <v>2</v>
       </c>
-      <c r="R8" s="33" t="s">
+      <c r="S8" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="S8" s="32" t="s">
-        <v>40</v>
-      </c>
       <c r="T8" s="32" t="s">
         <v>40</v>
       </c>
@@ -3628,18 +3695,18 @@
         <v>40</v>
       </c>
       <c r="Y8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z8" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="Z8" s="32" t="s">
-        <v>40</v>
-      </c>
       <c r="AA8" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="AB8" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC8" s="32" t="s">
+      <c r="AB8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC8" s="33" t="s">
         <v>40</v>
       </c>
       <c r="AD8" s="32" t="s">
@@ -3648,12 +3715,12 @@
       <c r="AE8" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="AF8" s="34" t="s">
+      <c r="AF8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG8" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="AG8" s="32" t="s">
-        <v>40</v>
-      </c>
       <c r="AH8" s="32" t="s">
         <v>40</v>
       </c>
@@ -3672,66 +3739,69 @@
       <c r="AM8" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="AN8" s="35" t="s">
+      <c r="AN8" s="32" t="s">
         <v>40</v>
       </c>
       <c r="AO8" s="35" t="s">
         <v>40</v>
       </c>
+      <c r="AP8" s="35" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="9" spans="2:41">
+    <row r="9" spans="2:42">
       <c r="B9" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="E9" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="12" t="b">
+      <c r="F9" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="F9" s="13">
+      <c r="G9" s="13">
         <v>1</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="H9" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="H9" s="15">
+      <c r="I9" s="15">
         <v>7</v>
       </c>
-      <c r="I9" s="16">
+      <c r="J9" s="16">
         <v>110</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="K9" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="15"/>
-      <c r="L9" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="M9" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="N9" s="19" t="s">
+      <c r="L9" s="15"/>
+      <c r="M9" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N9" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="O9" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="O9" s="19" t="s">
-        <v>40</v>
-      </c>
       <c r="P9" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="Q9" s="19">
+      <c r="Q9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="R9" s="19">
         <v>2</v>
       </c>
-      <c r="R9" s="20" t="s">
+      <c r="S9" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="S9" s="19" t="s">
-        <v>40</v>
-      </c>
       <c r="T9" s="19" t="s">
         <v>40</v>
       </c>
@@ -3748,18 +3818,18 @@
         <v>40</v>
       </c>
       <c r="Y9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z9" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="Z9" s="19" t="s">
-        <v>40</v>
-      </c>
       <c r="AA9" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="AB9" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC9" s="19" t="s">
+      <c r="AB9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC9" s="20" t="s">
         <v>40</v>
       </c>
       <c r="AD9" s="19" t="s">
@@ -3768,12 +3838,12 @@
       <c r="AE9" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="AF9" s="21" t="s">
+      <c r="AF9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG9" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="AG9" s="19" t="s">
-        <v>40</v>
-      </c>
       <c r="AH9" s="19" t="s">
         <v>40</v>
       </c>
@@ -3792,66 +3862,69 @@
       <c r="AM9" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="AN9" s="23" t="s">
+      <c r="AN9" s="19" t="s">
         <v>40</v>
       </c>
       <c r="AO9" s="23" t="s">
         <v>40</v>
       </c>
+      <c r="AP9" s="23" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="10" spans="2:41">
+    <row r="10" spans="2:42">
       <c r="B10" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="E10" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="25" t="b">
+      <c r="F10" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="F10" s="26">
+      <c r="G10" s="26">
         <v>1</v>
       </c>
-      <c r="G10" s="27" t="s">
+      <c r="H10" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="28">
+      <c r="I10" s="28">
         <v>8</v>
       </c>
-      <c r="I10" s="29">
+      <c r="J10" s="29">
         <v>250</v>
       </c>
-      <c r="J10" s="29" t="s">
+      <c r="K10" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="K10" s="28"/>
-      <c r="L10" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="M10" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="N10" s="32" t="s">
+      <c r="L10" s="28"/>
+      <c r="M10" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="O10" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="O10" s="32" t="s">
-        <v>40</v>
-      </c>
       <c r="P10" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="Q10" s="32">
+      <c r="Q10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="R10" s="32">
         <v>2</v>
       </c>
-      <c r="R10" s="33" t="s">
+      <c r="S10" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="S10" s="32" t="s">
-        <v>40</v>
-      </c>
       <c r="T10" s="32" t="s">
         <v>40</v>
       </c>
@@ -3868,18 +3941,18 @@
         <v>40</v>
       </c>
       <c r="Y10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z10" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="Z10" s="32" t="s">
-        <v>40</v>
-      </c>
       <c r="AA10" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="AB10" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC10" s="32" t="s">
+      <c r="AB10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC10" s="33" t="s">
         <v>40</v>
       </c>
       <c r="AD10" s="32" t="s">
@@ -3888,12 +3961,12 @@
       <c r="AE10" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="AF10" s="34" t="s">
+      <c r="AF10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG10" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="AG10" s="32" t="s">
-        <v>40</v>
-      </c>
       <c r="AH10" s="32" t="s">
         <v>40</v>
       </c>
@@ -3912,68 +3985,71 @@
       <c r="AM10" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="AN10" s="35" t="s">
+      <c r="AN10" s="32" t="s">
         <v>40</v>
       </c>
       <c r="AO10" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP10" s="35" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E3 E5">
+  <conditionalFormatting sqref="F3 F5">
     <cfRule type="containsText" dxfId="14" priority="17" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",E3)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",F3)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="13" priority="18" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",E3)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
+  <conditionalFormatting sqref="F4">
     <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",E4)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",F4)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",E4)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
+  <conditionalFormatting sqref="F6">
     <cfRule type="containsText" dxfId="10" priority="13" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",E6)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",F6)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="9" priority="14" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",E6)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7">
+  <conditionalFormatting sqref="F7">
     <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",E7)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",F7)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",E7)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F7)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
+  <conditionalFormatting sqref="F8">
     <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",E8)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",F8)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",E8)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E9">
+  <conditionalFormatting sqref="F9">
     <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",E9)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",F9)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",E9)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10">
+  <conditionalFormatting sqref="F10">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",E10)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",F10)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",E10)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>